<commit_message>
update to course project
</commit_message>
<xml_diff>
--- a/CourseProject/Trend Following Trading Project/Portfolio Return Data Yearly.xlsx
+++ b/CourseProject/Trend Following Trading Project/Portfolio Return Data Yearly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamp\Desktop\AdamPuntonRepository\CourseProject\Trend Following Trading Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813E177C-DEBD-491A-B45E-5F5007824020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6933D587-7219-42AE-B028-9AB63355DE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72DC65A9-3F7A-416B-8ADD-399F98D04260}"/>
+    <workbookView xWindow="7428" yWindow="2616" windowWidth="13056" windowHeight="8928" xr2:uid="{72DC65A9-3F7A-416B-8ADD-399F98D04260}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Mulvaney Capital Returns</t>
-  </si>
-  <si>
-    <t>Chesepeake Captial Returns</t>
-  </si>
-  <si>
     <t>AAPL</t>
   </si>
   <si>
@@ -66,6 +60,12 @@
   </si>
   <si>
     <t>^GSPC</t>
+  </si>
+  <si>
+    <t>Mulvaney Capital</t>
+  </si>
+  <si>
+    <t>Chesepeake Captial</t>
   </si>
 </sst>
 </file>
@@ -431,14 +431,13 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -446,31 +445,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1261,7 +1260,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664218A5-2783-48E1-A37C-C8F9C639754B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03806601-F679-4FDA-BFB3-4B8F8028B398}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>